<commit_message>
updated utilities script for correct reporting of MOEs.
</commit_message>
<xml_diff>
--- a/Support/BaseYear/validation/trn_validation_2017_20200601_fullrun.xlsx
+++ b/Support/BaseYear/validation/trn_validation_2017_20200601_fullrun.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Clients\Nashville\Tasks\Task9_ReCalibration\Validation\transit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Clients\Nashville\GitHub\ABM_TCAD8_TAZSPLIT\Support\BaseYear\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -10422,7 +10422,7 @@
   <dimension ref="A1:AX85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10747,7 +10747,7 @@
       </c>
       <c r="F9" s="122"/>
       <c r="G9" s="125">
-        <v>23765</v>
+        <v>23846</v>
       </c>
       <c r="H9" s="122"/>
       <c r="I9" s="122"/>
@@ -10769,7 +10769,7 @@
       <c r="F10" s="122"/>
       <c r="G10" s="128">
         <f>G8/G9</f>
-        <v>1.4796128760782663</v>
+        <v>1.4745869328189214</v>
       </c>
       <c r="H10" s="122"/>
       <c r="I10" s="122"/>

</xml_diff>